<commit_message>
Updates to make Cloud Plots work with new 2023 TriRvw output
</commit_message>
<xml_diff>
--- a/data/HistPE.xlsx
+++ b/data/HistPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfelletter\Documents\RW-RDF-Process-Plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B45AFB-72E0-472E-BB0E-EF926FEDDC5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ADC39B-B02C-433D-8E58-DDAC4DD92668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13110" yWindow="975" windowWidth="12150" windowHeight="21285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="2370" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
@@ -884,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FA3F15-F84C-4733-AC4D-279958C970B8}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,43 +1125,43 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1999</v>
+        <v>2019</v>
       </c>
       <c r="B22">
-        <v>1213.9399410000001</v>
+        <v>3608.74</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2000</v>
+        <v>2020</v>
       </c>
       <c r="B23">
-        <v>1196.119995</v>
+        <v>3582.21</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2001</v>
+        <v>2021</v>
       </c>
       <c r="B24">
-        <v>1177.369995</v>
+        <v>3537.33</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="B25">
-        <v>1152.130005</v>
+        <v>1213.9399410000001</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="B26">
-        <v>1139.119995</v>
+        <v>1196.119995</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="B27">
-        <v>1130.01</v>
+        <v>1177.369995</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="B28">
-        <v>1137.52</v>
+        <v>1152.130005</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="B29">
-        <v>1128.1199999999999</v>
+        <v>1139.119995</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="B30">
-        <v>1114.81</v>
+        <v>1130.01</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1224,10 +1224,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="B31">
-        <v>1110.97</v>
+        <v>1137.52</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1235,10 +1235,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B32">
-        <v>1096.3</v>
+        <v>1128.1199999999999</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="B33">
-        <v>1086.3</v>
+        <v>1114.81</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="B34">
-        <v>1132.83</v>
+        <v>1110.97</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="B35">
-        <v>1120.3599999999999</v>
+        <v>1096.3</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B36">
-        <v>1106.73</v>
+        <v>1086.3</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="B37">
-        <v>1087.79</v>
+        <v>1132.83</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1301,10 +1301,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="B38">
-        <v>1080.9100000000001</v>
+        <v>1120.3599999999999</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="B39">
-        <v>1080.82</v>
+        <v>1106.73</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="B40">
-        <v>1082.52</v>
+        <v>1087.79</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1334,49 +1334,82 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>2015</v>
+      </c>
+      <c r="B41">
+        <v>1080.9100000000001</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2016</v>
+      </c>
+      <c r="B42">
+        <v>1080.82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2017</v>
+      </c>
+      <c r="B43">
+        <v>1082.52</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>2018</v>
       </c>
-      <c r="B41">
+      <c r="B44">
         <v>1081.46</v>
       </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45">
+        <v>2019</v>
+      </c>
+      <c r="B45">
+        <v>1090.49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46">
+        <v>2020</v>
+      </c>
+      <c r="B46">
+        <v>1083.72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="A47">
+        <v>2021</v>
+      </c>
+      <c r="B47">
+        <v>1066.3900000000001</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,6 +1610,24 @@
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>